<commit_message>
Laser power up, grafik och design
</commit_message>
<xml_diff>
--- a/Dokumentation/Iteration v21/Iteration 6.xlsx
+++ b/Dokumentation/Iteration v21/Iteration 6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="58">
   <si>
     <t>Analys av föregående iteration</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Jag tänkte lägga in den sista power-up för att skjuta med plattan, skapa highscore lista, jobba lite med ljud, meka med kollisionen och fixa till designen så att applikationen ser snygg ut.</t>
+  </si>
+  <si>
+    <t>Påbörjat</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +938,7 @@
         <v>38</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
@@ -950,7 +953,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
@@ -965,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D29" s="4">
         <v>2.5</v>
@@ -980,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D30" s="4">
         <v>2.5</v>
@@ -1072,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D40" s="4">
         <v>1.5</v>
@@ -1089,12 +1092,14 @@
         <v>39</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D41" s="4">
         <v>3</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
@@ -1102,12 +1107,14 @@
         <v>45</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D42" s="4">
         <v>2</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -1222,12 +1229,14 @@
         <v>55</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D50" s="4">
         <v>4</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
@@ -1280,7 +1289,7 @@
       </c>
       <c r="E54" s="4">
         <f>SUM(E39:E53)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>